<commit_message>
Moved to .NET 4.8 (as 4.5 is no longer supported)
</commit_message>
<xml_diff>
--- a/ExcelFixture/ExcelFixtureTest/TestSheet.xlsx
+++ b/ExcelFixture/ExcelFixtureTest/TestSheet.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rik.Essenius\source\repos\essenius\FitNesseFitSharpExcel\ExcelFixture\ExcelFixtureTest\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C243532-D32C-45B3-B770-8C1C95B885D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="10500" windowHeight="7680"/>
+    <workbookView xWindow="38190" yWindow="1035" windowWidth="35220" windowHeight="19710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -66,14 +72,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -111,7 +120,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -183,7 +192,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -356,14 +365,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -374,25 +383,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{d0cb1e24-a0e2-4a4c-9340-733297c9cd7c}" enabled="1" method="Privileged" siteId="{db1e96a8-a3da-442a-930b-235cac24cd5c}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>